<commit_message>
Updated by VB & SB
Question 3 completed
</commit_message>
<xml_diff>
--- a/Output_Worst_Q3.xlsx
+++ b/Output_Worst_Q3.xlsx
@@ -495,28 +495,28 @@
         <v>13</v>
       </c>
       <c r="D2">
-        <v>161.7</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="E2">
-        <v>5240</v>
+        <v>1998</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>5239</v>
+        <v>1998</v>
       </c>
       <c r="H2">
-        <v>808641.98</v>
+        <v>356785.71</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>154.32</v>
+        <v>178.57</v>
       </c>
       <c r="K2">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -530,28 +530,28 @@
         <v>14</v>
       </c>
       <c r="D3">
-        <v>160.5</v>
+        <v>53.8</v>
       </c>
       <c r="E3">
-        <v>4878</v>
+        <v>1998</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>599</v>
       </c>
       <c r="G3">
-        <v>4877</v>
+        <v>1398</v>
       </c>
       <c r="H3">
-        <v>802302.63</v>
+        <v>376858.46</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>29.98</v>
       </c>
       <c r="J3">
-        <v>164.47</v>
+        <v>188.62</v>
       </c>
       <c r="K3">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -565,28 +565,28 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <v>198.1</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="E4">
-        <v>5942</v>
+        <v>1998</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>5942</v>
+        <v>1998</v>
       </c>
       <c r="H4">
-        <v>990333.33</v>
+        <v>356785.71</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>166.67</v>
+        <v>178.57</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -600,28 +600,28 @@
         <v>16</v>
       </c>
       <c r="D5">
-        <v>71.8</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="E5">
-        <v>2297</v>
+        <v>1998</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>2297</v>
+        <v>1998</v>
       </c>
       <c r="H5">
-        <v>358906.25</v>
+        <v>333000</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>156.25</v>
+        <v>166.67</v>
       </c>
       <c r="K5">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -635,28 +635,28 @@
         <v>17</v>
       </c>
       <c r="D6">
-        <v>63.8</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="E6">
-        <v>1992</v>
+        <v>1998</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1991</v>
+        <v>1998</v>
       </c>
       <c r="H6">
-        <v>319230.77</v>
+        <v>356785.71</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>160.26</v>
+        <v>178.57</v>
       </c>
       <c r="K6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -670,25 +670,25 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>77.90000000000001</v>
+        <v>53.8</v>
       </c>
       <c r="E7">
-        <v>2275</v>
+        <v>1998</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>599</v>
       </c>
       <c r="G7">
-        <v>2275</v>
+        <v>1398</v>
       </c>
       <c r="H7">
-        <v>389554.79</v>
+        <v>376858.46</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>29.98</v>
       </c>
       <c r="J7">
-        <v>171.23</v>
+        <v>188.62</v>
       </c>
       <c r="K7">
         <v>0.4</v>
@@ -705,28 +705,28 @@
         <v>19</v>
       </c>
       <c r="D8">
-        <v>137.3</v>
+        <v>58.3</v>
       </c>
       <c r="E8">
-        <v>5334</v>
+        <v>1998</v>
       </c>
       <c r="F8">
-        <v>1600</v>
+        <v>599</v>
       </c>
       <c r="G8">
-        <v>3734</v>
+        <v>1399</v>
       </c>
       <c r="H8">
-        <v>974397.0600000001</v>
+        <v>399278.33</v>
       </c>
       <c r="I8">
-        <v>30</v>
+        <v>29.98</v>
       </c>
       <c r="J8">
-        <v>182.68</v>
+        <v>199.84</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -740,28 +740,28 @@
         <v>20</v>
       </c>
       <c r="D9">
-        <v>110.9</v>
+        <v>53.8</v>
       </c>
       <c r="E9">
-        <v>3371</v>
+        <v>1998</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>599</v>
       </c>
       <c r="G9">
-        <v>3371</v>
+        <v>1398</v>
       </c>
       <c r="H9">
-        <v>554440.79</v>
+        <v>376858.46</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>29.98</v>
       </c>
       <c r="J9">
-        <v>164.47</v>
+        <v>188.62</v>
       </c>
       <c r="K9">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -775,28 +775,28 @@
         <v>21</v>
       </c>
       <c r="D10">
-        <v>116</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="E10">
-        <v>3759</v>
+        <v>1998</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>3759</v>
+        <v>1998</v>
       </c>
       <c r="H10">
-        <v>580092.59</v>
+        <v>356785.71</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>154.32</v>
+        <v>178.57</v>
       </c>
       <c r="K10">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -810,28 +810,28 @@
         <v>22</v>
       </c>
       <c r="D11">
-        <v>120.9</v>
+        <v>53.8</v>
       </c>
       <c r="E11">
-        <v>3529</v>
+        <v>1998</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>599</v>
       </c>
       <c r="G11">
-        <v>3529</v>
+        <v>1398</v>
       </c>
       <c r="H11">
-        <v>604280.8199999999</v>
+        <v>376858.46</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>29.98</v>
       </c>
       <c r="J11">
-        <v>171.23</v>
+        <v>188.62</v>
       </c>
       <c r="K11">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -845,28 +845,28 @@
         <v>23</v>
       </c>
       <c r="D12">
-        <v>110.3</v>
+        <v>58.3</v>
       </c>
       <c r="E12">
-        <v>4284</v>
+        <v>1998</v>
       </c>
       <c r="F12">
-        <v>1285</v>
+        <v>599</v>
       </c>
       <c r="G12">
-        <v>2998</v>
+        <v>1399</v>
       </c>
       <c r="H12">
-        <v>782586.76</v>
+        <v>399278.33</v>
       </c>
       <c r="I12">
-        <v>30</v>
+        <v>29.98</v>
       </c>
       <c r="J12">
-        <v>182.68</v>
+        <v>199.84</v>
       </c>
       <c r="K12">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -880,28 +880,28 @@
         <v>24</v>
       </c>
       <c r="D13">
-        <v>139.6</v>
+        <v>58.3</v>
       </c>
       <c r="E13">
-        <v>5183</v>
+        <v>1998</v>
       </c>
       <c r="F13">
-        <v>1554</v>
+        <v>599</v>
       </c>
       <c r="G13">
-        <v>3628</v>
+        <v>1399</v>
       </c>
       <c r="H13">
-        <v>977604.62</v>
+        <v>399278.33</v>
       </c>
       <c r="I13">
         <v>29.98</v>
       </c>
       <c r="J13">
-        <v>188.62</v>
+        <v>199.84</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -915,28 +915,28 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>152.1</v>
+        <v>42.8</v>
       </c>
       <c r="E14">
-        <v>4927</v>
+        <v>1998</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>799</v>
       </c>
       <c r="G14">
-        <v>4927</v>
+        <v>1199</v>
       </c>
       <c r="H14">
-        <v>696977.88</v>
+        <v>316114.88</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>39.99</v>
       </c>
       <c r="J14">
-        <v>141.46</v>
+        <v>158.22</v>
       </c>
       <c r="K14">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -950,28 +950,28 @@
         <v>14</v>
       </c>
       <c r="D15">
-        <v>51.9</v>
+        <v>46.1</v>
       </c>
       <c r="E15">
-        <v>2628</v>
+        <v>1998</v>
       </c>
       <c r="F15">
-        <v>1051</v>
+        <v>799</v>
       </c>
       <c r="G15">
-        <v>1577</v>
+        <v>1198</v>
       </c>
       <c r="H15">
-        <v>395410.42</v>
+        <v>331212.18</v>
       </c>
       <c r="I15">
         <v>39.99</v>
       </c>
       <c r="J15">
-        <v>150.46</v>
+        <v>165.77</v>
       </c>
       <c r="K15">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -985,28 +985,28 @@
         <v>15</v>
       </c>
       <c r="D16">
-        <v>59.5</v>
+        <v>42.8</v>
       </c>
       <c r="E16">
-        <v>2974</v>
+        <v>1998</v>
       </c>
       <c r="F16">
-        <v>1189</v>
+        <v>799</v>
       </c>
       <c r="G16">
-        <v>1785</v>
+        <v>1199</v>
       </c>
       <c r="H16">
-        <v>451058.33</v>
+        <v>316114.88</v>
       </c>
       <c r="I16">
-        <v>39.98</v>
+        <v>39.99</v>
       </c>
       <c r="J16">
-        <v>151.67</v>
+        <v>158.22</v>
       </c>
       <c r="K16">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1020,25 +1020,25 @@
         <v>16</v>
       </c>
       <c r="D17">
-        <v>73.09999999999999</v>
+        <v>40</v>
       </c>
       <c r="E17">
-        <v>2338</v>
+        <v>1998</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>799</v>
       </c>
       <c r="G17">
-        <v>2338</v>
+        <v>1199</v>
       </c>
       <c r="H17">
-        <v>334869.79</v>
+        <v>303030.56</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>39.99</v>
       </c>
       <c r="J17">
-        <v>143.23</v>
+        <v>151.67</v>
       </c>
       <c r="K17">
         <v>0.3</v>
@@ -1055,28 +1055,28 @@
         <v>17</v>
       </c>
       <c r="D18">
-        <v>128.8</v>
+        <v>42.8</v>
       </c>
       <c r="E18">
-        <v>4020</v>
+        <v>1998</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>799</v>
       </c>
       <c r="G18">
-        <v>4020</v>
+        <v>1199</v>
       </c>
       <c r="H18">
-        <v>590544.87</v>
+        <v>316114.88</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>39.99</v>
       </c>
       <c r="J18">
-        <v>146.9</v>
+        <v>158.22</v>
       </c>
       <c r="K18">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1090,28 +1090,28 @@
         <v>18</v>
       </c>
       <c r="D19">
-        <v>64.7</v>
+        <v>46.1</v>
       </c>
       <c r="E19">
-        <v>3147</v>
+        <v>1998</v>
       </c>
       <c r="F19">
-        <v>1258</v>
+        <v>799</v>
       </c>
       <c r="G19">
-        <v>1888</v>
+        <v>1198</v>
       </c>
       <c r="H19">
-        <v>485204</v>
+        <v>331212.18</v>
       </c>
       <c r="I19">
-        <v>39.97</v>
+        <v>39.99</v>
       </c>
       <c r="J19">
-        <v>154.18</v>
+        <v>165.77</v>
       </c>
       <c r="K19">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1125,28 +1125,28 @@
         <v>19</v>
       </c>
       <c r="D20">
-        <v>94.2</v>
+        <v>50</v>
       </c>
       <c r="E20">
-        <v>4271</v>
+        <v>1998</v>
       </c>
       <c r="F20">
-        <v>1708</v>
+        <v>799</v>
       </c>
       <c r="G20">
-        <v>2563</v>
+        <v>1198</v>
       </c>
       <c r="H20">
-        <v>688078.0600000001</v>
+        <v>348825.69</v>
       </c>
       <c r="I20">
         <v>39.99</v>
       </c>
       <c r="J20">
-        <v>161.1</v>
+        <v>174.59</v>
       </c>
       <c r="K20">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1160,28 +1160,28 @@
         <v>20</v>
       </c>
       <c r="D21">
-        <v>51.7</v>
+        <v>46.1</v>
       </c>
       <c r="E21">
-        <v>2620</v>
+        <v>1998</v>
       </c>
       <c r="F21">
-        <v>1048</v>
+        <v>799</v>
       </c>
       <c r="G21">
-        <v>1572</v>
+        <v>1198</v>
       </c>
       <c r="H21">
-        <v>394206.58</v>
+        <v>331212.18</v>
       </c>
       <c r="I21">
-        <v>40</v>
+        <v>39.99</v>
       </c>
       <c r="J21">
-        <v>150.46</v>
+        <v>165.77</v>
       </c>
       <c r="K21">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1195,28 +1195,28 @@
         <v>21</v>
       </c>
       <c r="D22">
-        <v>139.4</v>
+        <v>42.8</v>
       </c>
       <c r="E22">
-        <v>4517</v>
+        <v>1998</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>799</v>
       </c>
       <c r="G22">
-        <v>4517</v>
+        <v>1199</v>
       </c>
       <c r="H22">
-        <v>638978.91</v>
+        <v>316114.88</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>39.99</v>
       </c>
       <c r="J22">
-        <v>141.46</v>
+        <v>158.22</v>
       </c>
       <c r="K22">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1230,28 +1230,28 @@
         <v>22</v>
       </c>
       <c r="D23">
-        <v>85.40000000000001</v>
+        <v>46.1</v>
       </c>
       <c r="E23">
-        <v>4155</v>
+        <v>1998</v>
       </c>
       <c r="F23">
-        <v>1662</v>
+        <v>799</v>
       </c>
       <c r="G23">
-        <v>2492</v>
+        <v>1198</v>
       </c>
       <c r="H23">
-        <v>640609.9300000001</v>
+        <v>331212.18</v>
       </c>
       <c r="I23">
-        <v>40</v>
+        <v>39.99</v>
       </c>
       <c r="J23">
-        <v>154.18</v>
+        <v>165.77</v>
       </c>
       <c r="K23">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1265,28 +1265,28 @@
         <v>23</v>
       </c>
       <c r="D24">
-        <v>69.2</v>
+        <v>50</v>
       </c>
       <c r="E24">
-        <v>3137</v>
+        <v>1998</v>
       </c>
       <c r="F24">
-        <v>1254</v>
+        <v>799</v>
       </c>
       <c r="G24">
-        <v>1883</v>
+        <v>1198</v>
       </c>
       <c r="H24">
-        <v>505394.73</v>
+        <v>348825.69</v>
       </c>
       <c r="I24">
-        <v>39.97</v>
+        <v>39.99</v>
       </c>
       <c r="J24">
-        <v>161.11</v>
+        <v>174.59</v>
       </c>
       <c r="K24">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1300,28 +1300,28 @@
         <v>24</v>
       </c>
       <c r="D25">
-        <v>97.59999999999999</v>
+        <v>50</v>
       </c>
       <c r="E25">
-        <v>4227</v>
+        <v>1998</v>
       </c>
       <c r="F25">
-        <v>1690</v>
+        <v>799</v>
       </c>
       <c r="G25">
-        <v>2537</v>
+        <v>1198</v>
       </c>
       <c r="H25">
-        <v>700727.5600000001</v>
+        <v>348825.69</v>
       </c>
       <c r="I25">
-        <v>39.98</v>
+        <v>39.99</v>
       </c>
       <c r="J25">
-        <v>165.77</v>
+        <v>174.59</v>
       </c>
       <c r="K25">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1335,28 +1335,28 @@
         <v>13</v>
       </c>
       <c r="D26">
-        <v>35.9</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="E26">
-        <v>1162</v>
+        <v>1998</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
-        <v>1162</v>
+        <v>1998</v>
       </c>
       <c r="H26">
-        <v>158400.21</v>
+        <v>315160.71</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26">
-        <v>136.32</v>
+        <v>157.74</v>
       </c>
       <c r="K26">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1370,25 +1370,25 @@
         <v>14</v>
       </c>
       <c r="D27">
-        <v>64.7</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>1967</v>
+        <v>1998</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1998</v>
       </c>
       <c r="G27">
-        <v>1967</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <v>285775.77</v>
+        <v>319680</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J27">
-        <v>145.29</v>
+        <v>160</v>
       </c>
       <c r="K27">
         <v>0.3</v>
@@ -1405,25 +1405,25 @@
         <v>15</v>
       </c>
       <c r="D28">
-        <v>63.3</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="E28">
-        <v>1898</v>
+        <v>1998</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>1898</v>
+        <v>1998</v>
       </c>
       <c r="H28">
-        <v>279427.78</v>
+        <v>315160.71</v>
       </c>
       <c r="I28">
         <v>0</v>
       </c>
       <c r="J28">
-        <v>147.22</v>
+        <v>157.74</v>
       </c>
       <c r="K28">
         <v>0.3</v>
@@ -1440,25 +1440,25 @@
         <v>16</v>
       </c>
       <c r="D29">
-        <v>70.7</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="E29">
-        <v>2261</v>
+        <v>1998</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29">
-        <v>2261</v>
+        <v>1998</v>
       </c>
       <c r="H29">
-        <v>312065.1</v>
+        <v>294150</v>
       </c>
       <c r="I29">
         <v>0</v>
       </c>
       <c r="J29">
-        <v>138.02</v>
+        <v>147.22</v>
       </c>
       <c r="K29">
         <v>0.3</v>
@@ -1475,25 +1475,25 @@
         <v>17</v>
       </c>
       <c r="D30">
-        <v>65.09999999999999</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="E30">
-        <v>2030</v>
+        <v>1998</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
-        <v>2030</v>
+        <v>1998</v>
       </c>
       <c r="H30">
-        <v>287366.45</v>
+        <v>315160.71</v>
       </c>
       <c r="I30">
         <v>0</v>
       </c>
       <c r="J30">
-        <v>141.56</v>
+        <v>157.74</v>
       </c>
       <c r="K30">
         <v>0.3</v>
@@ -1510,28 +1510,28 @@
         <v>18</v>
       </c>
       <c r="D31">
-        <v>56.2</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>1642</v>
+        <v>1998</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>1998</v>
       </c>
       <c r="G31">
-        <v>1642</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>248361.87</v>
+        <v>319680</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J31">
-        <v>151.26</v>
+        <v>160</v>
       </c>
       <c r="K31">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1548,16 +1548,16 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>2489</v>
+        <v>1998</v>
       </c>
       <c r="F32">
-        <v>2489</v>
+        <v>1998</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>398240</v>
+        <v>319680</v>
       </c>
       <c r="I32">
         <v>100</v>
@@ -1566,7 +1566,7 @@
         <v>160</v>
       </c>
       <c r="K32">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1580,28 +1580,28 @@
         <v>20</v>
       </c>
       <c r="D33">
-        <v>82.09999999999999</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>2496</v>
+        <v>1998</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1998</v>
       </c>
       <c r="G33">
-        <v>2495</v>
+        <v>0</v>
       </c>
       <c r="H33">
-        <v>362631.58</v>
+        <v>319680</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J33">
-        <v>145.29</v>
+        <v>160</v>
       </c>
       <c r="K33">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1615,28 +1615,28 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <v>28.5</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="E34">
-        <v>922</v>
+        <v>1998</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34">
-        <v>922</v>
+        <v>1998</v>
       </c>
       <c r="H34">
-        <v>125684.16</v>
+        <v>315160.71</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34">
-        <v>136.32</v>
+        <v>157.74</v>
       </c>
       <c r="K34">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1650,28 +1650,28 @@
         <v>22</v>
       </c>
       <c r="D35">
-        <v>82.90000000000001</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>2421</v>
+        <v>1998</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>1998</v>
       </c>
       <c r="G35">
-        <v>2421</v>
+        <v>0</v>
       </c>
       <c r="H35">
-        <v>366190.07</v>
+        <v>319680</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J35">
-        <v>151.26</v>
+        <v>160</v>
       </c>
       <c r="K35">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1688,16 +1688,16 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>963</v>
+        <v>1998</v>
       </c>
       <c r="F36">
-        <v>963</v>
+        <v>1998</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36">
-        <v>154080</v>
+        <v>319680</v>
       </c>
       <c r="I36">
         <v>100</v>
@@ -1706,7 +1706,7 @@
         <v>160</v>
       </c>
       <c r="K36">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="37" spans="1:11">

</xml_diff>